<commit_message>
updated based on PR sheet
</commit_message>
<xml_diff>
--- a/Requirments/CAR_SRS .xlsx
+++ b/Requirments/CAR_SRS .xlsx
@@ -11,14 +11,20 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7miToNs+lmHIz71xAWNP1o20zBNBoA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mhwsd36kCkCAxUVC1dhpiJ8uB9+AQ=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="115">
+  <si>
+    <t>Car_ID</t>
+  </si>
+  <si>
+    <t>Functional Requirements</t>
+  </si>
   <si>
     <t>Car_NFR</t>
   </si>
@@ -26,23 +32,35 @@
     <t>Car_CR</t>
   </si>
   <si>
-    <t>Car_ID</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
     <t>Car_NFR_01</t>
   </si>
   <si>
-    <t>Functional Requirements</t>
-  </si>
-  <si>
-    <t>Car_SRS_01</t>
+    <t>CAR_CR_01</t>
   </si>
   <si>
     <t xml:space="preserve"> The performance SLA for this application is that the application shall response not exceed 10 seconds for 90
  percentile of the total requests done when the system is loaded with 500 concurrent users.</t>
+  </si>
+  <si>
+    <t>The user can register and login and land on the car listing page with number of currently available cars</t>
+  </si>
+  <si>
+    <t>Car_SRS_01</t>
+  </si>
+  <si>
+    <t>CAR_CR_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The user can search for cars based on different search criteria </t>
+  </si>
+  <si>
+    <t>CAR_CR_03</t>
+  </si>
+  <si>
+    <t>The user has the option to reserve a car from the available cars</t>
   </si>
   <si>
     <r>
@@ -66,11 +84,12 @@
       <rPr>
         <b/>
       </rPr>
-      <t>Role:Guest</t>
+      <t xml:space="preserve">Role:Guest
+</t>
     </r>
     <r>
       <t xml:space="preserve">
-The guest can search for cars colors from drop down list after clicking on color button from home page of car web app.  
+The guest can search for cars colors by choosing the desired color from the drop down list found in the home page 
 </t>
     </r>
   </si>
@@ -141,12 +160,6 @@
     <t>Car_SRS_07</t>
   </si>
   <si>
-    <t>CAR_CR_01</t>
-  </si>
-  <si>
-    <t>The user can register and login and land on the car listing page with number of currently available cars</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -159,13 +172,7 @@
     </r>
   </si>
   <si>
-    <t>CAR_CR_02</t>
-  </si>
-  <si>
     <t>Car_SRS_08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The user can search for cars based on different search criteria </t>
   </si>
   <si>
     <r>
@@ -181,12 +188,6 @@
     </r>
   </si>
   <si>
-    <t>CAR_CR_03</t>
-  </si>
-  <si>
-    <t>The user has the option to reserve a car from the available cars</t>
-  </si>
-  <si>
     <t>Car_SRS_09</t>
   </si>
   <si>
@@ -214,7 +215,7 @@
     </r>
     <r>
       <t xml:space="preserve">
-If the guest tries to register without entering the username or the password in registration page, error msg will be displayed as " All the fields are mandatory, please try again"</t>
+If the guest tries to register without entering the username or the password in registration page, error msg will be displayed as "  Please fill out this field"</t>
     </r>
   </si>
   <si>
@@ -314,9 +315,8 @@
     </r>
     <r>
       <t xml:space="preserve">
-The user can view all cars details and it may includes( the model year, engine CC , gear transmission , condition(new or used) , 
-kilometers(for used cars) when he/she clicks on "see more" button under car image from user home page .
-</t>
+The user can view all cars details after clicking on see more button which redirects him/her to the car details page that may include( the model year, engine CC , 
+gear transmission , condition(new or used) , kilometers(for used cars)</t>
     </r>
   </si>
   <si>
@@ -331,7 +331,7 @@
 </t>
     </r>
     <r>
-      <t>The user can search for cars colors from drop down list after clicking on color button from home page of car web app.</t>
+      <t>The guest can search for cars colors by choosing the desired color from the drop down list found in the home page.</t>
     </r>
   </si>
   <si>
@@ -409,9 +409,7 @@
     </r>
     <r>
       <t xml:space="preserve">
-The user can reserve the car he/she wants after clicking on "see more" button from user home page under the car image and description and the user will be redirected to
-"see more" page to reserve the car after clicking on "reserve" button.
-</t>
+The user can reserve a car by clicking on " reserve" button found in the car details page so the car status will be converted from free to reserved.</t>
     </r>
   </si>
   <si>
@@ -474,7 +472,7 @@
     </r>
     <r>
       <t xml:space="preserve">
-If the user tries to login without entering the username or the password, error msg will be displayed "All the fields are mandatory, please try again"           
+If the user tries to login without entering the username or the password, error msg will be displayed "Please fill out this field"           
             </t>
     </r>
   </si>
@@ -583,7 +581,7 @@
     </r>
     <r>
       <t xml:space="preserve"> 
-Admin can remove car(s) from the system using add car tab in the admin home web page.</t>
+Admin can remove car(s) from the system using delete car button found under each car in the "all cars" page.</t>
     </r>
   </si>
   <si>
@@ -598,7 +596,7 @@
     </r>
     <r>
       <t xml:space="preserve"> 
-Admin can update each car status from reserved to sold using the admin home web page.</t>
+Admin can change car status from reserved to sold from the status drop list found under each car in " all cars" page</t>
     </r>
   </si>
   <si>
@@ -614,71 +612,18 @@
     </r>
     <r>
       <t xml:space="preserve">
-Admin can update each car status from reserved to free using the admin home web page.</t>
+Admin can change car status from reserved to free from the status drop list found under each car in " all cars" page</t>
     </r>
   </si>
   <si>
     <t>Car_SRS_40</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-      </rPr>
-      <t>Role:Admin</t>
-    </r>
-    <r>
-      <t xml:space="preserve">
-Admin can search and view all free cars using the admin home web page after clicking on All cars button.  </t>
-    </r>
+    <t xml:space="preserve">Role:Admin 
+The car shall be removed from search page once it's status be "reserved" but the admin can change its status to free if the car is not confirmed to be bought within 24 hours </t>
   </si>
   <si>
     <t>Car_SRS_41</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-      </rPr>
-      <t xml:space="preserve">Role:Admin </t>
-    </r>
-    <r>
-      <t xml:space="preserve">
-Admin can search and view all reserved cars using the admin home web page after clicking on all cars button .  </t>
-    </r>
-  </si>
-  <si>
-    <t>Car_SRS_42</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-      </rPr>
-      <t xml:space="preserve">Role:Admin  </t>
-    </r>
-    <r>
-      <t xml:space="preserve">
-Admin can search and view all sold cars using the admin home web page after clicking on all cars button.  </t>
-    </r>
-  </si>
-  <si>
-    <t>Car_SRS_43</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-      </rPr>
-      <t>Role:Admin</t>
-    </r>
-    <r>
-      <t xml:space="preserve"> 
-Admin remove car from search page after 24 hours if it is confirmed to be bought.  </t>
-    </r>
-  </si>
-  <si>
-    <t>Car_SRS_44</t>
   </si>
   <si>
     <r>
@@ -693,88 +638,63 @@
     </r>
   </si>
   <si>
-    <t>Car_SRS_45</t>
+    <t>Car_SRS_42</t>
   </si>
   <si>
     <t xml:space="preserve">The user home page shall contain scrollable list of cars, search bar, my profile button, logout button, home button,about us button, reserved cars button
  and see more button under each car image.                                                                                                                                                                                                        </t>
   </si>
   <si>
-    <t>Car_SRS_46</t>
-  </si>
-  <si>
-    <t>About us tab shall redirect user to about us page contain all information about car web app.</t>
-  </si>
-  <si>
-    <t>Car_SRS_47</t>
-  </si>
-  <si>
-    <t>If Reservation button is pressed it shall change car status from free to reserved and removed the reserved car from search page.</t>
-  </si>
-  <si>
-    <t>Car_SRS_48</t>
+    <t>Car_SRS_43</t>
+  </si>
+  <si>
+    <t>If Reservation button found in car details page is pressed it shall change car status from free to reserved and removed the reserved car from search page.</t>
+  </si>
+  <si>
+    <t>Car_SRS_44</t>
   </si>
   <si>
     <t>Registration page shall contain "Register" button if it's pressed after filling all fields following the above mentioned constraints and the entered data doesn't exist 
 in the system's database, the browser shall be redirected to the user home page. else the wrong fields shall be surrounded with the error message describing what is wrong</t>
   </si>
   <si>
+    <t>Car_SRS_45</t>
+  </si>
+  <si>
+    <t>The user home page shall contain "profile" button, once it's pressed, profile page shall be loaded</t>
+  </si>
+  <si>
+    <t>Car_SRS_46</t>
+  </si>
+  <si>
+    <t>Profile page shall review all the current logged in user information will be displayed but only address and phone number are editable.</t>
+  </si>
+  <si>
+    <t>Car_SRS_47</t>
+  </si>
+  <si>
+    <t>In the profile page the user can edit phone number and address fields only</t>
+  </si>
+  <si>
+    <t>Car_SRS_48</t>
+  </si>
+  <si>
+    <t>In the profile page there are two edit buttons beside phone number and address fields</t>
+  </si>
+  <si>
+    <t>Car_SRS_49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin home page shall contain "All Cars" button, once it pressed All cars (free,reserved and sold) shall be previewed </t>
+  </si>
+  <si>
     <t>Car_SRS_50</t>
   </si>
   <si>
-    <t>The user home page shall contain "profile" button, once it's pressed, profile page shall be loaded</t>
+    <t xml:space="preserve">Admin home page shall contain "Reserved Cars" button, once it's pressed reserved cars shall be previewed </t>
   </si>
   <si>
     <t>Car_SRS_51</t>
-  </si>
-  <si>
-    <t>profile page shall preview all the current logged in user information (address and phone number).</t>
-  </si>
-  <si>
-    <t>Car_SRS_52</t>
-  </si>
-  <si>
-    <t>In the profile page the user can edit phone number and address fields only</t>
-  </si>
-  <si>
-    <t>Car_SRS_53</t>
-  </si>
-  <si>
-    <t>In the profile page there are two edit buttons beside phone number and address fields</t>
-  </si>
-  <si>
-    <t>Car_SRS_54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Admin home page shall contain "All Cars" button, once it pressed All cars (free,reserved and sold) shall be previewed </t>
-  </si>
-  <si>
-    <t>Car_SRS_55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Admin home page shall contain "Reserved Cars" button, once it's pressed reserved cars shall be previewed </t>
-  </si>
-  <si>
-    <t>Car_SRS_56</t>
-  </si>
-  <si>
-    <t>Admin home page shall contain "Users" button, once it's pressed, users web page shall be loaded</t>
-  </si>
-  <si>
-    <t>Car_SRS_57</t>
-  </si>
-  <si>
-    <t>Users web page shall preview all users in matrix view, under each user cell, there is a "delete" button once it's pressed, the selected user shall be deleted 
-from the database after confirming the alert message</t>
-  </si>
-  <si>
-    <t>Car_SRS_58</t>
-  </si>
-  <si>
-    <t>Admin home page shall contain "Add user" button, once it's pressed, registration page shall be loaded</t>
-  </si>
-  <si>
-    <t>Car_SRS_59</t>
   </si>
   <si>
     <t xml:space="preserve">Admin home page shal contain "Add cars"button, once it's pressed, add cars page shall be loaded contains(car type, car model, car price, and car description) fields. </t>
@@ -792,11 +712,11 @@
     </font>
     <font>
       <b/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="12.0"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <color rgb="FFFFFFFF"/>
     </font>
     <font/>
     <font>
@@ -855,22 +775,22 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -947,178 +867,178 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" ht="53.25" customHeight="1">
-      <c r="A2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>8</v>
+      <c r="A2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" ht="43.5" customHeight="1">
-      <c r="A3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>10</v>
+      <c r="A3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" ht="43.5" customHeight="1">
-      <c r="A4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>12</v>
+      <c r="A4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" ht="43.5" customHeight="1">
-      <c r="A5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>14</v>
+      <c r="A5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" ht="43.5" customHeight="1">
-      <c r="A6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>16</v>
+      <c r="A6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" ht="43.5" customHeight="1">
-      <c r="A7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>18</v>
+      <c r="A7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" ht="43.5" customHeight="1">
-      <c r="A8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>22</v>
+      <c r="A8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="9" ht="43.5" customHeight="1">
-      <c r="A9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>26</v>
+      <c r="A9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10" ht="43.5" customHeight="1">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="7" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="11" ht="53.25" customHeight="1">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="12" ht="53.25" customHeight="1">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="13" ht="43.5" customHeight="1">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14" ht="43.5" customHeight="1">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="7" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="15" ht="43.5" customHeight="1">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="7" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="16" ht="43.5" customHeight="1">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="7" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="17" ht="43.5" customHeight="1">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="7" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="18" ht="43.5" customHeight="1">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="7" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="19" ht="52.5" customHeight="1">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="7" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="20" ht="45.75" customHeight="1">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="7" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="21" ht="58.5" customHeight="1">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="7" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="22" ht="45.75" customHeight="1">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="7" t="s">
         <v>54</v>
       </c>
       <c r="C22" s="9"/>
@@ -1149,10 +1069,10 @@
       <c r="AB22" s="9"/>
     </row>
     <row r="23" ht="45.75" customHeight="1">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="7" t="s">
         <v>56</v>
       </c>
       <c r="C23" s="9"/>
@@ -1183,10 +1103,10 @@
       <c r="AB23" s="9"/>
     </row>
     <row r="24" ht="45.75" customHeight="1">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="7" t="s">
         <v>58</v>
       </c>
       <c r="C24" s="9"/>
@@ -1217,10 +1137,10 @@
       <c r="AB24" s="9"/>
     </row>
     <row r="25" ht="45.75" customHeight="1">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="7" t="s">
         <v>60</v>
       </c>
       <c r="C25" s="9"/>
@@ -1251,10 +1171,10 @@
       <c r="AB25" s="9"/>
     </row>
     <row r="26" ht="45.75" customHeight="1">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="7" t="s">
         <v>62</v>
       </c>
       <c r="C26" s="9"/>
@@ -1285,10 +1205,10 @@
       <c r="AB26" s="9"/>
     </row>
     <row r="27" ht="63.0" customHeight="1">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="7" t="s">
         <v>64</v>
       </c>
       <c r="C27" s="9"/>
@@ -1319,10 +1239,10 @@
       <c r="AB27" s="9"/>
     </row>
     <row r="28" ht="45.75" customHeight="1">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="7" t="s">
         <v>66</v>
       </c>
       <c r="C28" s="10"/>
@@ -1353,10 +1273,10 @@
       <c r="AB28" s="9"/>
     </row>
     <row r="29" ht="45.75" customHeight="1">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="7" t="s">
         <v>68</v>
       </c>
       <c r="C29" s="9"/>
@@ -1387,7 +1307,7 @@
       <c r="AB29" s="9"/>
     </row>
     <row r="30" ht="55.5" customHeight="1">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="5" t="s">
         <v>69</v>
       </c>
       <c r="B30" s="11" t="s">
@@ -1421,10 +1341,10 @@
       <c r="AB30" s="9"/>
     </row>
     <row r="31" ht="54.75" customHeight="1">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="7" t="s">
         <v>72</v>
       </c>
       <c r="C31" s="9"/>
@@ -1455,10 +1375,10 @@
       <c r="AB31" s="9"/>
     </row>
     <row r="32" ht="45.75" customHeight="1">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="7" t="s">
         <v>74</v>
       </c>
       <c r="C32" s="9"/>
@@ -1489,7 +1409,7 @@
       <c r="AB32" s="9"/>
     </row>
     <row r="33" ht="45.75" customHeight="1">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="5" t="s">
         <v>75</v>
       </c>
       <c r="B33" s="12" t="s">
@@ -1523,7 +1443,7 @@
       <c r="AB33" s="9"/>
     </row>
     <row r="34" ht="38.25" customHeight="1">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="5" t="s">
         <v>77</v>
       </c>
       <c r="B34" s="13" t="s">
@@ -1531,7 +1451,7 @@
       </c>
     </row>
     <row r="35" ht="38.25" customHeight="1">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="5" t="s">
         <v>79</v>
       </c>
       <c r="B35" s="13" t="s">
@@ -1539,7 +1459,7 @@
       </c>
     </row>
     <row r="36" ht="36.0" customHeight="1">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="5" t="s">
         <v>81</v>
       </c>
       <c r="B36" s="14" t="s">
@@ -1573,7 +1493,7 @@
       <c r="AB36" s="9"/>
     </row>
     <row r="37" ht="45.75" customHeight="1">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="5" t="s">
         <v>83</v>
       </c>
       <c r="B37" s="15" t="s">
@@ -1607,7 +1527,7 @@
       <c r="AB37" s="9"/>
     </row>
     <row r="38" ht="45.75" customHeight="1">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="5" t="s">
         <v>85</v>
       </c>
       <c r="B38" s="15" t="s">
@@ -1641,7 +1561,7 @@
       <c r="AB38" s="9"/>
     </row>
     <row r="39" ht="45.75" customHeight="1">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="5" t="s">
         <v>87</v>
       </c>
       <c r="B39" s="15" t="s">
@@ -1675,7 +1595,7 @@
       <c r="AB39" s="9"/>
     </row>
     <row r="40" ht="45.75" customHeight="1">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="5" t="s">
         <v>89</v>
       </c>
       <c r="B40" s="15" t="s">
@@ -1709,7 +1629,7 @@
       <c r="AB40" s="9"/>
     </row>
     <row r="41" ht="45.75" customHeight="1">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="5" t="s">
         <v>91</v>
       </c>
       <c r="B41" s="15" t="s">
@@ -1743,7 +1663,7 @@
       <c r="AB41" s="9"/>
     </row>
     <row r="42" ht="45.75" customHeight="1">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="5" t="s">
         <v>93</v>
       </c>
       <c r="B42" s="15" t="s">
@@ -1776,8 +1696,8 @@
       <c r="AA42" s="9"/>
       <c r="AB42" s="9"/>
     </row>
-    <row r="43" ht="45.75" customHeight="1">
-      <c r="A43" s="4" t="s">
+    <row r="43" ht="32.25" customHeight="1">
+      <c r="A43" s="5" t="s">
         <v>95</v>
       </c>
       <c r="B43" s="15" t="s">
@@ -1810,263 +1730,131 @@
       <c r="AA43" s="9"/>
       <c r="AB43" s="9"/>
     </row>
-    <row r="44" ht="45.75" customHeight="1">
-      <c r="A44" s="4" t="s">
+    <row r="44" ht="19.5" customHeight="1">
+      <c r="A44" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
-      <c r="J44" s="9"/>
-      <c r="K44" s="9"/>
-      <c r="L44" s="9"/>
-      <c r="M44" s="9"/>
-      <c r="N44" s="9"/>
-      <c r="O44" s="9"/>
-      <c r="P44" s="9"/>
-      <c r="Q44" s="9"/>
-      <c r="R44" s="9"/>
-      <c r="S44" s="9"/>
-      <c r="T44" s="9"/>
-      <c r="U44" s="9"/>
-      <c r="V44" s="9"/>
-      <c r="W44" s="9"/>
-      <c r="X44" s="9"/>
-      <c r="Y44" s="9"/>
-      <c r="Z44" s="9"/>
-      <c r="AA44" s="9"/>
-      <c r="AB44" s="9"/>
-    </row>
-    <row r="45" ht="45.75" customHeight="1">
-      <c r="A45" s="4" t="s">
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="16"/>
+      <c r="J44" s="16"/>
+      <c r="K44" s="16"/>
+      <c r="L44" s="16"/>
+      <c r="M44" s="16"/>
+      <c r="N44" s="16"/>
+      <c r="O44" s="16"/>
+      <c r="P44" s="16"/>
+      <c r="Q44" s="16"/>
+      <c r="R44" s="16"/>
+      <c r="S44" s="16"/>
+      <c r="T44" s="16"/>
+      <c r="U44" s="16"/>
+      <c r="V44" s="16"/>
+      <c r="W44" s="16"/>
+      <c r="X44" s="16"/>
+      <c r="Y44" s="16"/>
+      <c r="Z44" s="16"/>
+      <c r="AA44" s="16"/>
+      <c r="AB44" s="16"/>
+    </row>
+    <row r="45" ht="43.5" customHeight="1">
+      <c r="A45" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="9"/>
-      <c r="J45" s="9"/>
-      <c r="K45" s="9"/>
-      <c r="L45" s="9"/>
-      <c r="M45" s="9"/>
-      <c r="N45" s="9"/>
-      <c r="O45" s="9"/>
-      <c r="P45" s="9"/>
-      <c r="Q45" s="9"/>
-      <c r="R45" s="9"/>
-      <c r="S45" s="9"/>
-      <c r="T45" s="9"/>
-      <c r="U45" s="9"/>
-      <c r="V45" s="9"/>
-      <c r="W45" s="9"/>
-      <c r="X45" s="9"/>
-      <c r="Y45" s="9"/>
-      <c r="Z45" s="9"/>
-      <c r="AA45" s="9"/>
-      <c r="AB45" s="9"/>
-    </row>
-    <row r="46" ht="32.25" customHeight="1">
-      <c r="A46" s="4" t="s">
+    </row>
+    <row r="46" ht="21.75" customHeight="1">
+      <c r="A46" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B46" s="15" t="s">
+      <c r="B46" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
-      <c r="J46" s="9"/>
-      <c r="K46" s="9"/>
-      <c r="L46" s="9"/>
-      <c r="M46" s="9"/>
-      <c r="N46" s="9"/>
-      <c r="O46" s="9"/>
-      <c r="P46" s="9"/>
-      <c r="Q46" s="9"/>
-      <c r="R46" s="9"/>
-      <c r="S46" s="9"/>
-      <c r="T46" s="9"/>
-      <c r="U46" s="9"/>
-      <c r="V46" s="9"/>
-      <c r="W46" s="9"/>
-      <c r="X46" s="9"/>
-      <c r="Y46" s="9"/>
-      <c r="Z46" s="9"/>
-      <c r="AA46" s="9"/>
-      <c r="AB46" s="9"/>
-    </row>
-    <row r="47" ht="24.0" customHeight="1">
-      <c r="A47" s="4" t="s">
+    </row>
+    <row r="47" ht="21.75" customHeight="1">
+      <c r="A47" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
-      <c r="H47" s="16"/>
-      <c r="I47" s="16"/>
-      <c r="J47" s="16"/>
-      <c r="K47" s="16"/>
-      <c r="L47" s="16"/>
-      <c r="M47" s="16"/>
-      <c r="N47" s="16"/>
-      <c r="O47" s="16"/>
-      <c r="P47" s="16"/>
-      <c r="Q47" s="16"/>
-      <c r="R47" s="16"/>
-      <c r="S47" s="16"/>
-      <c r="T47" s="16"/>
-      <c r="U47" s="16"/>
-      <c r="V47" s="16"/>
-      <c r="W47" s="16"/>
-      <c r="X47" s="16"/>
-      <c r="Y47" s="16"/>
-      <c r="Z47" s="16"/>
-      <c r="AA47" s="16"/>
-      <c r="AB47" s="16"/>
-    </row>
-    <row r="48" ht="19.5" customHeight="1">
-      <c r="A48" s="4" t="s">
+    </row>
+    <row r="48" ht="21.75" customHeight="1">
+      <c r="A48" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C48" s="16"/>
-      <c r="D48" s="16"/>
-      <c r="E48" s="16"/>
-      <c r="F48" s="16"/>
-      <c r="G48" s="16"/>
-      <c r="H48" s="16"/>
-      <c r="I48" s="16"/>
-      <c r="J48" s="16"/>
-      <c r="K48" s="16"/>
-      <c r="L48" s="16"/>
-      <c r="M48" s="16"/>
-      <c r="N48" s="16"/>
-      <c r="O48" s="16"/>
-      <c r="P48" s="16"/>
-      <c r="Q48" s="16"/>
-      <c r="R48" s="16"/>
-      <c r="S48" s="16"/>
-      <c r="T48" s="16"/>
-      <c r="U48" s="16"/>
-      <c r="V48" s="16"/>
-      <c r="W48" s="16"/>
-      <c r="X48" s="16"/>
-      <c r="Y48" s="16"/>
-      <c r="Z48" s="16"/>
-      <c r="AA48" s="16"/>
-      <c r="AB48" s="16"/>
-    </row>
-    <row r="49" ht="43.5" customHeight="1">
-      <c r="A49" s="4" t="s">
+    </row>
+    <row r="49" ht="21.75" customHeight="1">
+      <c r="A49" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B49" s="7" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="50" ht="21.75" customHeight="1">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="7" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="51" ht="21.75" customHeight="1">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B51" s="7" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="52" ht="21.75" customHeight="1">
-      <c r="A52" s="4" t="s">
+    <row r="52" ht="15.75" customHeight="1">
+      <c r="A52" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="B52" s="17" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="53" ht="21.75" customHeight="1">
-      <c r="A53" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="54" ht="21.75" customHeight="1">
-      <c r="A54" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="55" ht="21.75" customHeight="1">
-      <c r="A55" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>120</v>
-      </c>
+    <row r="53" ht="15.75" customHeight="1">
+      <c r="A53" s="18"/>
+      <c r="B53" s="19"/>
+    </row>
+    <row r="54" ht="15.75" customHeight="1">
+      <c r="A54" s="18"/>
+      <c r="B54" s="19"/>
+    </row>
+    <row r="55" ht="15.75" customHeight="1">
+      <c r="A55" s="18"/>
+      <c r="B55" s="19"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>122</v>
-      </c>
+      <c r="A56" s="18"/>
+      <c r="B56" s="19"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>124</v>
-      </c>
+      <c r="A57" s="18"/>
+      <c r="B57" s="19"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>126</v>
-      </c>
+      <c r="A58" s="18"/>
+      <c r="B58" s="19"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="B59" s="17" t="s">
-        <v>128</v>
-      </c>
+      <c r="A59" s="18"/>
+      <c r="B59" s="19"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="18"/>
@@ -2777,31 +2565,24 @@
       <c r="B236" s="19"/>
     </row>
     <row r="237" ht="15.75" customHeight="1">
-      <c r="A237" s="18"/>
       <c r="B237" s="19"/>
     </row>
     <row r="238" ht="15.75" customHeight="1">
-      <c r="A238" s="18"/>
       <c r="B238" s="19"/>
     </row>
     <row r="239" ht="15.75" customHeight="1">
-      <c r="A239" s="18"/>
       <c r="B239" s="19"/>
     </row>
     <row r="240" ht="15.75" customHeight="1">
-      <c r="A240" s="18"/>
       <c r="B240" s="19"/>
     </row>
     <row r="241" ht="15.75" customHeight="1">
-      <c r="A241" s="18"/>
       <c r="B241" s="19"/>
     </row>
     <row r="242" ht="15.75" customHeight="1">
-      <c r="A242" s="18"/>
       <c r="B242" s="19"/>
     </row>
     <row r="243" ht="15.75" customHeight="1">
-      <c r="A243" s="18"/>
       <c r="B243" s="19"/>
     </row>
     <row r="244" ht="15.75" customHeight="1">
@@ -5050,27 +4831,6 @@
     </row>
     <row r="992" ht="15.75" customHeight="1">
       <c r="B992" s="19"/>
-    </row>
-    <row r="993" ht="15.75" customHeight="1">
-      <c r="B993" s="19"/>
-    </row>
-    <row r="994" ht="15.75" customHeight="1">
-      <c r="B994" s="19"/>
-    </row>
-    <row r="995" ht="15.75" customHeight="1">
-      <c r="B995" s="19"/>
-    </row>
-    <row r="996" ht="15.75" customHeight="1">
-      <c r="B996" s="19"/>
-    </row>
-    <row r="997" ht="15.75" customHeight="1">
-      <c r="B997" s="19"/>
-    </row>
-    <row r="998" ht="15.75" customHeight="1">
-      <c r="B998" s="19"/>
-    </row>
-    <row r="999" ht="15.75" customHeight="1">
-      <c r="B999" s="19"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -5093,55 +4853,55 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
     </row>
     <row r="2" ht="33.0" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" ht="31.5" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" ht="31.5" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1"/>
@@ -6161,48 +5921,48 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
     </row>
     <row r="2" ht="33.0" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="7"/>
+      <c r="C2" s="6"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
     </row>
     <row r="3" ht="31.5" customHeight="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="7"/>
+      <c r="B3" s="6"/>
     </row>
     <row r="4" ht="31.5" customHeight="1"/>
     <row r="5" ht="15.75" customHeight="1"/>

</xml_diff>